<commit_message>
Update: updated for Fall-25 & Spring-26 - version 1.0
</commit_message>
<xml_diff>
--- a/uploads/xlsx/Timetable SE Department (Fall-25 & Spring-26) Version-1.0.xlsx
+++ b/uploads/xlsx/Timetable SE Department (Fall-25 & Spring-26) Version-1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPythonStuff\Superior Academic Tool\uploads\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F828374-8C01-4F81-8474-BEEF0D2C87FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A725408D-ABD7-4F34-A557-BE579135D502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="577" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1087,14 +1087,6 @@
 Mr. Adeel </t>
   </si>
   <si>
-    <t>Knowledge Representation &amp; Reasoning 
-BSAI-6A/BSAI-6C</t>
-  </si>
-  <si>
-    <t>Knowledge Representation &amp; Reasoning 
-BSAI-6B</t>
-  </si>
-  <si>
     <t xml:space="preserve">Computer Organization &amp; Assembly Language (Lab)
 BSAI-6B
 Mr. Hafiz Asad Ali </t>
@@ -1655,6 +1647,16 @@
     <t xml:space="preserve">Big Data Analytics 
 BSDS-5A/BSDS-7A
 Mr. Usman Baig </t>
+  </si>
+  <si>
+    <t>Knowledge Representation &amp; Reasoning 
+BSAI-6A/BSAI-6C
+N/A</t>
+  </si>
+  <si>
+    <t>Knowledge Representation &amp; Reasoning 
+BSAI-6B
+N/A</t>
   </si>
 </sst>
 </file>
@@ -5325,7 +5327,7 @@
         <v>94</v>
       </c>
       <c r="H7" s="189" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I7" s="190"/>
       <c r="J7" s="348"/>
@@ -5359,11 +5361,11 @@
       </c>
       <c r="E8" s="356"/>
       <c r="F8" s="357" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G8" s="195"/>
       <c r="H8" s="187" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I8" s="188"/>
       <c r="J8" s="139"/>
@@ -5397,7 +5399,7 @@
         <v>133</v>
       </c>
       <c r="F9" s="357" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G9" s="195"/>
       <c r="H9" s="187" t="s">
@@ -5446,7 +5448,7 @@
       </c>
       <c r="H10" s="147"/>
       <c r="I10" s="193" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J10" s="193"/>
       <c r="K10" s="144"/>
@@ -5475,11 +5477,11 @@
       </c>
       <c r="C11" s="290"/>
       <c r="D11" s="267" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E11" s="297"/>
       <c r="F11" s="191" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G11" s="192"/>
       <c r="H11" s="191" t="s">
@@ -5517,7 +5519,7 @@
       </c>
       <c r="E12" s="224"/>
       <c r="F12" s="191" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G12" s="192"/>
       <c r="H12" s="360" t="s">
@@ -5551,18 +5553,18 @@
       </c>
       <c r="C13" s="290"/>
       <c r="D13" s="194" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E13" s="195"/>
       <c r="F13" s="90" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G13" s="300" t="s">
         <v>88</v>
       </c>
       <c r="H13" s="300"/>
       <c r="I13" s="184" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J13" s="185"/>
       <c r="K13" s="117"/>
@@ -5635,7 +5637,7 @@
       </c>
       <c r="E15" s="370"/>
       <c r="F15" s="298" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G15" s="197"/>
       <c r="H15" s="323" t="s">
@@ -5673,7 +5675,7 @@
       </c>
       <c r="E16" s="185"/>
       <c r="F16" s="187" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G16" s="188"/>
       <c r="H16" s="187" t="s">
@@ -5681,7 +5683,7 @@
       </c>
       <c r="I16" s="188"/>
       <c r="J16" s="294" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K16" s="209"/>
       <c r="L16" s="2"/>
@@ -5721,7 +5723,7 @@
       </c>
       <c r="I17" s="192"/>
       <c r="J17" s="187" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K17" s="206"/>
       <c r="L17" s="2"/>
@@ -5749,15 +5751,15 @@
       </c>
       <c r="C18" s="290"/>
       <c r="D18" s="186" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E18" s="224"/>
       <c r="F18" s="207" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G18" s="208"/>
       <c r="H18" s="187" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I18" s="188"/>
       <c r="J18" s="147"/>
@@ -5787,11 +5789,11 @@
       </c>
       <c r="C19" s="291"/>
       <c r="D19" s="231" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E19" s="295"/>
       <c r="F19" s="296" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G19" s="295"/>
       <c r="H19" s="201"/>
@@ -5917,7 +5919,7 @@
         <v>74</v>
       </c>
       <c r="H22" s="220" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I22" s="342"/>
       <c r="J22" s="313"/>
@@ -5957,7 +5959,7 @@
         <v>58</v>
       </c>
       <c r="H23" s="220" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I23" s="342"/>
       <c r="J23" s="207"/>
@@ -5991,7 +5993,7 @@
       </c>
       <c r="E24" s="194"/>
       <c r="F24" s="252" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G24" s="252"/>
       <c r="H24" s="193" t="s">
@@ -6027,7 +6029,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="307" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E25" s="188"/>
       <c r="F25" s="193" t="s">
@@ -6035,7 +6037,7 @@
       </c>
       <c r="G25" s="193"/>
       <c r="H25" s="193" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I25" s="200"/>
       <c r="J25" s="22"/>
@@ -6073,11 +6075,11 @@
       </c>
       <c r="G26" s="188"/>
       <c r="H26" s="243" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I26" s="367"/>
       <c r="J26" s="207" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K26" s="209"/>
       <c r="L26" s="2"/>
@@ -6105,7 +6107,7 @@
       </c>
       <c r="C27" s="229"/>
       <c r="D27" s="188" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E27" s="193"/>
       <c r="F27" s="319" t="s">
@@ -6145,7 +6147,7 @@
       </c>
       <c r="C28" s="229"/>
       <c r="D28" s="188" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E28" s="193"/>
       <c r="F28" s="320" t="s">
@@ -6156,7 +6158,7 @@
         <v>127</v>
       </c>
       <c r="I28" s="359" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J28" s="197"/>
       <c r="K28" s="122"/>
@@ -6185,7 +6187,7 @@
       </c>
       <c r="C29" s="229"/>
       <c r="D29" s="188" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E29" s="187"/>
       <c r="F29" s="319" t="s">
@@ -6193,11 +6195,11 @@
       </c>
       <c r="G29" s="200"/>
       <c r="H29" s="193" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I29" s="193"/>
       <c r="J29" s="188" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K29" s="240"/>
       <c r="L29" s="2"/>
@@ -6269,11 +6271,11 @@
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="193" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G31" s="200"/>
       <c r="H31" s="351" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I31" s="352"/>
       <c r="J31" s="353"/>
@@ -6307,11 +6309,11 @@
       </c>
       <c r="E32" s="342"/>
       <c r="F32" s="327" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G32" s="281"/>
       <c r="H32" s="216" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I32" s="216"/>
       <c r="J32" s="337"/>
@@ -6343,11 +6345,11 @@
         <v>11</v>
       </c>
       <c r="D33" s="341" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E33" s="218"/>
       <c r="F33" s="327" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G33" s="342"/>
       <c r="H33" s="327" t="s">
@@ -6383,11 +6385,11 @@
         <v>15</v>
       </c>
       <c r="D34" s="231" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E34" s="295"/>
       <c r="F34" s="296" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G34" s="336"/>
       <c r="H34" s="339" t="s">
@@ -6511,11 +6513,11 @@
         <v>109</v>
       </c>
       <c r="F37" s="238" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G37" s="239"/>
       <c r="H37" s="196" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I37" s="197"/>
       <c r="J37" s="204"/>
@@ -6545,7 +6547,7 @@
       </c>
       <c r="C38" s="330"/>
       <c r="D38" s="186" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E38" s="186"/>
       <c r="F38" s="22" t="s">
@@ -6633,17 +6635,17 @@
       </c>
       <c r="E40" s="186"/>
       <c r="F40" s="22" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G40" s="142" t="s">
         <v>119</v>
       </c>
       <c r="H40" s="187" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I40" s="188"/>
       <c r="J40" s="187" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K40" s="206"/>
       <c r="L40" s="2"/>
@@ -6671,7 +6673,7 @@
       </c>
       <c r="C41" s="330"/>
       <c r="D41" s="186" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E41" s="215"/>
       <c r="F41" s="187" t="s">
@@ -6713,7 +6715,7 @@
       </c>
       <c r="E42" s="186"/>
       <c r="F42" s="187" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G42" s="188"/>
       <c r="H42" s="343" t="s">
@@ -6756,11 +6758,11 @@
         <v>126</v>
       </c>
       <c r="G43" s="193" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H43" s="200"/>
       <c r="I43" s="274" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J43" s="344"/>
       <c r="K43" s="117"/>
@@ -6821,11 +6823,11 @@
       </c>
       <c r="C45" s="330"/>
       <c r="D45" s="198" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E45" s="199"/>
       <c r="F45" s="272" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G45" s="273"/>
       <c r="H45" s="193" t="s">
@@ -6859,7 +6861,7 @@
       </c>
       <c r="C46" s="330"/>
       <c r="D46" s="299" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E46" s="300"/>
       <c r="F46" s="236" t="s">
@@ -6905,11 +6907,11 @@
       </c>
       <c r="G47" s="200"/>
       <c r="H47" s="193" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I47" s="200"/>
       <c r="J47" s="311" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K47" s="312"/>
       <c r="L47" s="2"/>
@@ -6941,7 +6943,7 @@
       </c>
       <c r="E48" s="200"/>
       <c r="F48" s="193" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G48" s="200"/>
       <c r="H48" s="193" t="s">
@@ -6977,15 +6979,15 @@
         <v>11</v>
       </c>
       <c r="D49" s="193" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E49" s="200"/>
       <c r="F49" s="193" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G49" s="200"/>
       <c r="H49" s="193" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I49" s="302"/>
       <c r="J49" s="145"/>
@@ -7024,11 +7026,11 @@
         <v>64</v>
       </c>
       <c r="G50" s="316" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H50" s="317"/>
       <c r="I50" s="182" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J50" s="182"/>
       <c r="K50" s="124"/>
@@ -7141,15 +7143,15 @@
         <v>11</v>
       </c>
       <c r="D53" s="265" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E53" s="266"/>
       <c r="F53" s="309" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G53" s="310"/>
       <c r="H53" s="187" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I53" s="188"/>
       <c r="J53" s="147"/>
@@ -7186,11 +7188,11 @@
         <v>60</v>
       </c>
       <c r="G54" s="193" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H54" s="200"/>
       <c r="I54" s="187" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J54" s="188"/>
       <c r="K54" s="140"/>
@@ -7234,7 +7236,7 @@
         <v>129</v>
       </c>
       <c r="I55" s="274" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J55" s="275"/>
       <c r="K55" s="117"/>
@@ -7277,11 +7279,11 @@
         <v>71</v>
       </c>
       <c r="H56" s="187" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I56" s="188"/>
       <c r="J56" s="187" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="K56" s="206"/>
       <c r="L56" s="2"/>
@@ -7321,7 +7323,7 @@
       </c>
       <c r="I57" s="200"/>
       <c r="J57" s="193" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K57" s="240"/>
       <c r="L57" s="2"/>
@@ -7349,7 +7351,7 @@
       </c>
       <c r="C58" s="200"/>
       <c r="D58" s="187" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E58" s="188"/>
       <c r="F58" s="22" t="s">
@@ -7359,11 +7361,11 @@
         <v>91</v>
       </c>
       <c r="H58" s="187" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I58" s="188"/>
       <c r="J58" s="241" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K58" s="242"/>
       <c r="L58" s="2"/>
@@ -7391,7 +7393,7 @@
       </c>
       <c r="C59" s="200"/>
       <c r="D59" s="193" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E59" s="200"/>
       <c r="F59" s="193" t="s">
@@ -7399,7 +7401,7 @@
       </c>
       <c r="G59" s="200"/>
       <c r="H59" s="187" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I59" s="188"/>
       <c r="J59" s="226" t="s">
@@ -7431,7 +7433,7 @@
       </c>
       <c r="C60" s="200"/>
       <c r="D60" s="193" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E60" s="200"/>
       <c r="F60" s="22" t="s">
@@ -7473,7 +7475,7 @@
       </c>
       <c r="C61" s="200"/>
       <c r="D61" s="187" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E61" s="188"/>
       <c r="F61" s="314" t="s">
@@ -7591,15 +7593,15 @@
         <v>31</v>
       </c>
       <c r="D64" s="193" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E64" s="200"/>
       <c r="F64" s="193" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G64" s="200"/>
       <c r="H64" s="193" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I64" s="200"/>
       <c r="J64" s="46"/>
@@ -7803,7 +7805,7 @@
       </c>
       <c r="E69" s="216"/>
       <c r="F69" s="223" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G69" s="215"/>
       <c r="H69" s="245"/>
@@ -7837,7 +7839,7 @@
       </c>
       <c r="C70" s="229"/>
       <c r="D70" s="220" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E70" s="221"/>
       <c r="F70" s="193" t="s">
@@ -7846,7 +7848,7 @@
       <c r="G70" s="187"/>
       <c r="H70" s="245"/>
       <c r="I70" s="222" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J70" s="222"/>
       <c r="K70" s="117"/>
@@ -7875,7 +7877,7 @@
       </c>
       <c r="C71" s="230"/>
       <c r="D71" s="220" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E71" s="221"/>
       <c r="F71" s="42" t="s">
@@ -7955,7 +7957,7 @@
       </c>
       <c r="C73" s="229"/>
       <c r="D73" s="217" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E73" s="218"/>
       <c r="F73" s="269" t="s">
@@ -7964,7 +7966,7 @@
       <c r="G73" s="213"/>
       <c r="H73" s="245"/>
       <c r="I73" s="214" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J73" s="215"/>
       <c r="K73" s="117"/>
@@ -8044,7 +8046,7 @@
       <c r="G75" s="216"/>
       <c r="H75" s="245"/>
       <c r="I75" s="214" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J75" s="215"/>
       <c r="K75" s="117"/>
@@ -8073,16 +8075,16 @@
       </c>
       <c r="C76" s="229"/>
       <c r="D76" s="186" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E76" s="225"/>
       <c r="F76" s="223" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G76" s="215"/>
       <c r="H76" s="245"/>
       <c r="I76" s="186" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J76" s="215"/>
       <c r="K76" s="117"/>
@@ -8151,12 +8153,12 @@
       </c>
       <c r="E78" s="263"/>
       <c r="F78" s="223" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G78" s="215"/>
       <c r="H78" s="245"/>
       <c r="I78" s="186" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J78" s="215"/>
       <c r="K78" s="117"/>
@@ -8217,7 +8219,7 @@
       </c>
       <c r="C80" s="230"/>
       <c r="D80" s="186" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E80" s="263"/>
       <c r="F80" s="223" t="s">
@@ -8255,7 +8257,7 @@
         <v>11</v>
       </c>
       <c r="D81" s="243" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E81" s="257"/>
       <c r="F81" s="212" t="s">
@@ -8264,7 +8266,7 @@
       <c r="G81" s="213"/>
       <c r="H81" s="245"/>
       <c r="I81" s="233" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J81" s="215"/>
       <c r="K81" s="117"/>
@@ -8295,16 +8297,16 @@
         <v>15</v>
       </c>
       <c r="D82" s="305" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E82" s="306"/>
       <c r="F82" s="182" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G82" s="183"/>
       <c r="H82" s="246"/>
       <c r="I82" s="231" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J82" s="232"/>
       <c r="K82" s="118"/>
@@ -36074,7 +36076,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36125,7 +36127,7 @@
         <v>149</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F3" s="169"/>
     </row>
@@ -36139,7 +36141,7 @@
         <v>158</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F4" s="170"/>
     </row>
@@ -36150,7 +36152,7 @@
       </c>
       <c r="C5" s="131"/>
       <c r="D5" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>152</v>
@@ -36165,10 +36167,10 @@
       <c r="C6" s="376"/>
       <c r="D6" s="11"/>
       <c r="E6" s="10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F6" s="169" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36192,7 +36194,7 @@
       </c>
       <c r="C8" s="377"/>
       <c r="D8" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>160</v>
@@ -36255,7 +36257,7 @@
         <v>203</v>
       </c>
       <c r="F12" s="172" t="s">
-        <v>207</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36309,7 +36311,7 @@
       </c>
       <c r="C16" s="131"/>
       <c r="D16" s="10" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>157</v>
@@ -36326,10 +36328,10 @@
         <v>162</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F17" s="169" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36354,10 +36356,10 @@
       <c r="C19" s="376"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F19" s="169" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36387,7 +36389,7 @@
         <v>183</v>
       </c>
       <c r="F21" s="169" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="66" x14ac:dyDescent="0.25">
@@ -36417,7 +36419,7 @@
         <v>206</v>
       </c>
       <c r="F23" s="169" t="s">
-        <v>208</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="66" x14ac:dyDescent="0.25">

</xml_diff>